<commit_message>
Added EnergySaving lib and code
</commit_message>
<xml_diff>
--- a/Data Translation.xlsx
+++ b/Data Translation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F030AA17-9731-43E5-B2EB-B8304C252D2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD10A112-6A65-4213-B166-AF64FDDD6A17}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" xr2:uid="{9C82DF01-607F-407C-B968-7F6BB654470A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>HEX</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>ID 900 081000009472</t>
+  </si>
+  <si>
+    <t>HEX 20D4526D11 = DEC 141001125137</t>
   </si>
 </sst>
 </file>
@@ -531,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AC4C85-8D2F-4D0E-A648-4A808950A492}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,10 +551,12 @@
     <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="11" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.77734375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="15" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="59.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -583,7 +588,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>10</v>
       </c>
@@ -598,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1000100</v>
       </c>
@@ -630,8 +635,20 @@
       <c r="L3" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="1">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>110000</v>
       </c>
@@ -659,8 +676,18 @@
         <v>2</v>
       </c>
       <c r="L4" s="16"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="1">
+        <v>31</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="16"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1000100</v>
       </c>
@@ -688,8 +715,18 @@
         <v>3</v>
       </c>
       <c r="L5" s="16"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="1">
+        <v>44</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>110110</v>
       </c>
@@ -717,8 +754,18 @@
         <v>9</v>
       </c>
       <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="1">
+        <v>36</v>
+      </c>
+      <c r="N6" s="1">
+        <v>6</v>
+      </c>
+      <c r="O6" s="1">
+        <v>4</v>
+      </c>
+      <c r="P6" s="16"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>110010</v>
       </c>
@@ -746,8 +793,18 @@
         <v>7</v>
       </c>
       <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="1">
+        <v>32</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5</v>
+      </c>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>110101</v>
       </c>
@@ -775,8 +832,18 @@
         <v>8</v>
       </c>
       <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="1">
+        <v>35</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1">
+        <v>2</v>
+      </c>
+      <c r="P8" s="16"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>110100</v>
       </c>
@@ -804,8 +871,18 @@
         <v>0</v>
       </c>
       <c r="L9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="1">
+        <v>34</v>
+      </c>
+      <c r="N9" s="1">
+        <v>4</v>
+      </c>
+      <c r="O9" s="1">
+        <v>6</v>
+      </c>
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1000100</v>
       </c>
@@ -833,8 +910,18 @@
         <v>7</v>
       </c>
       <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="1">
+        <v>44</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" s="16"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>110000</v>
       </c>
@@ -862,8 +949,18 @@
         <v>0</v>
       </c>
       <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="1">
+        <v>30</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>110010</v>
       </c>
@@ -891,8 +988,18 @@
         <v>0</v>
       </c>
       <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="1">
+        <v>32</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1</v>
+      </c>
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>111001</v>
       </c>
@@ -924,8 +1031,20 @@
       <c r="L13" s="16">
         <v>900</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="1">
+        <v>39</v>
+      </c>
+      <c r="N13" s="1">
+        <v>9</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="16">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1000100</v>
       </c>
@@ -953,8 +1072,18 @@
         <v>3</v>
       </c>
       <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="1">
+        <v>33</v>
+      </c>
+      <c r="N14" s="1">
+        <v>3</v>
+      </c>
+      <c r="O14" s="1">
+        <v>3</v>
+      </c>
+      <c r="P14" s="16"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>110011</v>
       </c>
@@ -982,8 +1111,18 @@
         <v>8</v>
       </c>
       <c r="L15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="1">
+        <v>44</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>110000</v>
       </c>
@@ -1011,8 +1150,18 @@
         <v>4</v>
       </c>
       <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="1">
+        <v>30</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>9</v>
+      </c>
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>110000</v>
       </c>
@@ -1032,8 +1181,11 @@
       <c r="J17" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>110001</v>
       </c>
@@ -1053,8 +1205,11 @@
       <c r="J18" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M18" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>110000</v>
       </c>
@@ -1075,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>110000</v>
       </c>
@@ -1096,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>110000</v>
       </c>
@@ -1117,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>110000</v>
       </c>
@@ -1138,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>110001</v>
       </c>
@@ -1159,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>110001</v>
       </c>
@@ -1180,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>110001</v>
       </c>
@@ -1201,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>110000</v>
       </c>
@@ -1222,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>110000</v>
       </c>
@@ -1243,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>110000</v>
       </c>
@@ -1264,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>1101</v>
       </c>
@@ -1279,7 +1434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>11110010</v>
       </c>
@@ -1294,7 +1449,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>11</v>
       </c>
@@ -1310,7 +1465,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="P3:P12"/>
+    <mergeCell ref="P13:P16"/>
     <mergeCell ref="L3:L12"/>
     <mergeCell ref="L13:L16"/>
     <mergeCell ref="F13:F16"/>

</xml_diff>